<commit_message>
update report and print
</commit_message>
<xml_diff>
--- a/Registration Response Kids Lab.xlsx
+++ b/Registration Response Kids Lab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\kidslab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kidslab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABF4FA1-F99E-465A-A283-1FB3F8A5ED6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59107F4-1D85-44EE-877D-8B3382AF2428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -405,11 +405,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -425,7 +425,7 @@
     <col min="11" max="15" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +457,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44042.244837905091</v>
       </c>
@@ -485,8 +485,9 @@
       <c r="J2" s="6">
         <v>44013</v>
       </c>
+      <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44042.246549293981</v>
       </c>
@@ -515,7 +516,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44042.252935763885</v>
       </c>
@@ -544,7 +545,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44042.256216585651</v>
       </c>
@@ -573,7 +574,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44042.257032638889</v>
       </c>
@@ -602,7 +603,7 @@
         <v>44013</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44042.257932141205</v>
       </c>

</xml_diff>